<commit_message>
change buy in time due
</commit_message>
<xml_diff>
--- a/[NAME] SB50 Prop bet 2016.xlsx
+++ b/[NAME] SB50 Prop bet 2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P_Hlawitschka\Desktop\Peter\Bets\Super bowl betting sheets\2016 TEP Super Bowl\Master sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\itsfinenow\hlawitschka.github.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -182,28 +182,6 @@
   </si>
   <si>
     <t>User: PeterH</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Buy-in is 25 Wotmans, winner take all. Payment </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> spreadsheets must be submitted by 8:00pm on Saturday. Payment information below.</t>
-    </r>
   </si>
   <si>
     <t>Boy or Girl</t>
@@ -456,6 +434,28 @@
   </si>
   <si>
     <t>Chris Paul assists on Feb 7th</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Buy-in is 25 Wotmans, winner take all. Payment </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> spreadsheets must be submitted by noon on Saturday. Payment information below.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1270,7 +1270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1284,7 +1286,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -1303,7 +1305,7 @@
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1325,7 +1327,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
@@ -1336,7 +1338,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
@@ -1347,7 +1349,7 @@
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B14" s="44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -1357,7 +1359,7 @@
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B16" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -1367,27 +1369,27 @@
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B18" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B19" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B20" s="44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B21" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B22" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1490,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -1506,13 +1508,13 @@
       <c r="B4" s="55"/>
       <c r="C4" s="56"/>
       <c r="L4" s="69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M4" s="69"/>
     </row>
     <row r="5" spans="1:27" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="66"/>
       <c r="D5" s="66"/>
@@ -1563,7 +1565,7 @@
         <v>33</v>
       </c>
       <c r="Y7" s="41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1597,7 +1599,7 @@
       <c r="I9" s="18"/>
       <c r="L9" s="7"/>
       <c r="M9" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -1641,19 +1643,19 @@
     <row r="11" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="16"/>
       <c r="I11" s="22"/>
       <c r="L11" s="7"/>
       <c r="M11" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -1699,7 +1701,7 @@
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -1727,7 +1729,7 @@
       <c r="I14" s="21"/>
       <c r="L14" s="7"/>
       <c r="M14" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -1781,7 +1783,7 @@
       <c r="I16" s="21"/>
       <c r="L16" s="7"/>
       <c r="M16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -1833,7 +1835,7 @@
       <c r="I18" s="22"/>
       <c r="L18" s="7"/>
       <c r="M18" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -1853,7 +1855,7 @@
       <c r="J19" s="5"/>
       <c r="L19" s="7"/>
       <c r="M19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -1882,7 +1884,7 @@
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -1909,7 +1911,7 @@
       <c r="I21" s="21"/>
       <c r="L21" s="8"/>
       <c r="M21" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
@@ -1949,7 +1951,7 @@
       <c r="H23" s="14"/>
       <c r="I23" s="21"/>
       <c r="L23" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
@@ -1969,7 +1971,7 @@
     <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1981,7 +1983,7 @@
       <c r="I24" s="21"/>
       <c r="L24" s="7"/>
       <c r="M24" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -1998,7 +2000,7 @@
     <row r="25" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -2010,7 +2012,7 @@
       <c r="I25" s="22"/>
       <c r="L25" s="7"/>
       <c r="M25" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -2030,7 +2032,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
       <c r="L26" s="57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M26" s="58"/>
       <c r="N26" s="58"/>
@@ -2060,7 +2062,7 @@
       </c>
       <c r="L27" s="7"/>
       <c r="M27" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
@@ -2077,7 +2079,7 @@
     <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -2089,7 +2091,7 @@
       <c r="I28" s="21"/>
       <c r="L28" s="7"/>
       <c r="M28" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -2106,7 +2108,7 @@
     <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
@@ -2118,7 +2120,7 @@
       <c r="I29" s="32"/>
       <c r="L29" s="7"/>
       <c r="M29" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -2135,7 +2137,7 @@
     <row r="30" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24"/>
       <c r="C30" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -2147,7 +2149,7 @@
       <c r="I30" s="28"/>
       <c r="L30" s="8"/>
       <c r="M30" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
@@ -2164,7 +2166,7 @@
     <row r="31" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="47"/>
       <c r="C31" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="48"/>
       <c r="E31" s="48"/>
@@ -2181,7 +2183,7 @@
     <row r="32" spans="2:22" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -2212,7 +2214,7 @@
     <row r="33" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -2224,7 +2226,7 @@
       <c r="I33" s="22"/>
       <c r="L33" s="7"/>
       <c r="M33" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
@@ -2242,7 +2244,7 @@
       <c r="I34" s="18"/>
       <c r="L34" s="7"/>
       <c r="M34" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
@@ -2256,22 +2258,22 @@
     </row>
     <row r="35" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L35" s="8"/>
       <c r="M35" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
@@ -2310,7 +2312,7 @@
       <c r="H37" s="14"/>
       <c r="I37" s="21"/>
       <c r="L37" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M37" s="11"/>
       <c r="N37" s="11"/>
@@ -2320,11 +2322,11 @@
       <c r="R37" s="11"/>
       <c r="S37" s="11"/>
       <c r="T37" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U37" s="12"/>
       <c r="V37" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.2">
@@ -2340,7 +2342,7 @@
       <c r="I38" s="21"/>
       <c r="L38" s="7"/>
       <c r="M38" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
@@ -2365,7 +2367,7 @@
       <c r="I39" s="21"/>
       <c r="L39" s="8"/>
       <c r="M39" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
@@ -2446,7 +2448,7 @@
     <row r="43" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L43" s="7"/>
       <c r="M43" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
@@ -2460,18 +2462,18 @@
     </row>
     <row r="44" spans="2:22" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H44" s="12"/>
       <c r="I44" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L44" s="7"/>
       <c r="M44" s="6" t="s">
@@ -2490,7 +2492,7 @@
     <row r="45" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -2500,7 +2502,7 @@
       <c r="I45" s="15"/>
       <c r="L45" s="8"/>
       <c r="M45" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
@@ -2515,7 +2517,7 @@
     <row r="46" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -2559,13 +2561,13 @@
       <c r="L49" s="8"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O49" s="45" t="s">
         <v>32</v>
       </c>
       <c r="P49" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q49" s="45" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
clarification on TD bets
</commit_message>
<xml_diff>
--- a/[NAME] SB50 Prop bet 2016.xlsx
+++ b/[NAME] SB50 Prop bet 2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
   <si>
     <t>Time</t>
   </si>
@@ -456,6 +456,12 @@
       </rPr>
       <t xml:space="preserve"> spreadsheets must be submitted by noon on Saturday. Payment information below.</t>
     </r>
+  </si>
+  <si>
+    <t>- The TD scoring bets (lines 25, 32, and 33) are based on the person who crosses the plane with the ball. That is, Peyton throwing for a TD doesn't count towards the white TD total</t>
+  </si>
+  <si>
+    <t>- However, for the QB player TDs (lines 28 and 30), thrown touchdowns DO count. Sorry about the confusion</t>
   </si>
 </sst>
 </file>
@@ -1268,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,93 +1353,108 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
       <c r="B14" s="44" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
       <c r="B15" s="44" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
       <c r="B16" s="44" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B17" s="44" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B18" s="44" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B19" s="44" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B20" s="44" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B21" s="44" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B22" s="44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B23" s="44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B24" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B25" s="44" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J29" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="33" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
@@ -1445,6 +1466,9 @@
     <row r="39" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="40" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="41" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="42" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="43" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="44" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D6:I6"/>
@@ -1458,7 +1482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>